<commit_message>
added specialty column to conformance table
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Environmental.xlsx
+++ b/docs/StructureDefinition-Environmental.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.3.6</t>
+    <t>0.4.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-08-15T13:55:23-06:00</t>
+    <t>2022-10-14T11:08:00-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>